<commit_message>
[IMP] Odoo 14 bank statement import
</commit_message>
<xml_diff>
--- a/om_account_bank_statement_import/sample_files/Import_Sample.xlsx
+++ b/om_account_bank_statement_import/sample_files/Import_Sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t xml:space="preserve">odoo mates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KWD</t>
   </si>
   <si>
     <t xml:space="preserve">Test 2</t>
@@ -62,6 +65,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -150,14 +154,14 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.78"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
@@ -192,19 +196,25 @@
       <c r="D2" s="0" t="n">
         <v>30</v>
       </c>
+      <c r="E2" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>40</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[IMP] reference in bank statement import
</commit_message>
<xml_diff>
--- a/om_account_bank_statement_import/sample_files/Import_Sample.xlsx
+++ b/om_account_bank_statement_import/sample_files/Import_Sample.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -28,6 +28,9 @@
     <t xml:space="preserve">Label</t>
   </si>
   <si>
+    <t xml:space="preserve">Reference</t>
+  </si>
+  <si>
     <t xml:space="preserve">Partner</t>
   </si>
   <si>
@@ -43,6 +46,9 @@
     <t xml:space="preserve">Test 1</t>
   </si>
   <si>
+    <t xml:space="preserve">Ref 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">odoo mates</t>
   </si>
   <si>
@@ -50,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">Test 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ref 2</t>
   </si>
 </sst>
 </file>
@@ -60,7 +69,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -81,6 +90,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,12 +139,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -151,19 +169,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="23.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -182,39 +200,48 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="0" t="n">
         <v>30</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>8</v>
+      <c r="F2" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="0" t="n">
+      <c r="E3" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>8</v>
+      <c r="F3" s="0" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>